<commit_message>
updated rebills and tires
</commit_message>
<xml_diff>
--- a/Rebill Pricing.xlsx
+++ b/Rebill Pricing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rushenterprises-my.sharepoint.com/personal/tuinderj_rushenterprises_com/Documents/Documents/SAP/SAP GUI/OneDrive Scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="118" documentId="8_{BA206BEA-BD8A-43D4-881F-890D9BCEB148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7579ED5F-4878-4216-AAEA-473EB0DB7224}"/>
+  <xr:revisionPtr revIDLastSave="127" documentId="8_{BA206BEA-BD8A-43D4-881F-890D9BCEB148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7435E226-4B92-43F9-AAC0-592B18426594}"/>
   <bookViews>
-    <workbookView xWindow="3375" yWindow="2460" windowWidth="27375" windowHeight="15435" xr2:uid="{1175D497-24F9-4868-9FA2-452FB0DE9A36}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{1175D497-24F9-4868-9FA2-452FB0DE9A36}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer Pricing" sheetId="1" r:id="rId1"/>
@@ -133,6 +133,18 @@
   </cellStyles>
   <dxfs count="15">
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -141,33 +153,21 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -203,33 +203,33 @@
     <tableColumn id="1" xr3:uid="{1BAE1BB9-5F82-4FE5-8828-511749738EE3}" name="Customer Name (Reference Only)" dataDxfId="13"/>
     <tableColumn id="2" xr3:uid="{B7897F1D-9F85-4537-BF22-BBA89E008D8A}" name="Customer Number" dataDxfId="12"/>
     <tableColumn id="3" xr3:uid="{69EFBF72-9AF5-4396-A811-267C0AC32B95}" name="Labor Rate" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{6C156DED-34DC-45E0-A2E7-C56236F36FA0}" name="Parts Markup" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{3F16856B-35DC-429C-9CDE-CA0FCEAF8FCA}" name="Parts Markup Cap" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{6C156DED-34DC-45E0-A2E7-C56236F36FA0}" name="Parts Markup" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{3F16856B-35DC-429C-9CDE-CA0FCEAF8FCA}" name="Parts Markup Cap" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2D3A599C-1216-4874-B044-A4922D481D18}" name="Table24" displayName="Table24" ref="A1:D13" totalsRowShown="0" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2D3A599C-1216-4874-B044-A4922D481D18}" name="Table24" displayName="Table24" ref="A1:D13" totalsRowShown="0" dataDxfId="8">
   <autoFilter ref="A1:D13" xr:uid="{2D3A599C-1216-4874-B044-A4922D481D18}"/>
   <tableColumns count="4">
-    <tableColumn id="2" xr3:uid="{0DCAC784-C852-431F-BF76-9D125CA20B97}" name="Unit Number (no dashes)" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{C20AEE42-F28D-4823-9F08-D2DE0E0FD307}" name="Labor Rate" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{D1B3C960-14D1-467A-8308-2473D0201BFF}" name="Parts Markup" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{3FA69D63-1508-415E-AEA4-3F2E9EB884BA}" name="Parts Markup Cap" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{0DCAC784-C852-431F-BF76-9D125CA20B97}" name="Unit Number (no dashes)" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{C20AEE42-F28D-4823-9F08-D2DE0E0FD307}" name="Labor Rate" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{D1B3C960-14D1-467A-8308-2473D0201BFF}" name="Parts Markup" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{3FA69D63-1508-415E-AEA4-3F2E9EB884BA}" name="Parts Markup Cap" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3FB93657-E6D3-447F-9D9A-FF03D845A830}" name="Table1" displayName="Table1" ref="A1:C3" totalsRowShown="0" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3FB93657-E6D3-447F-9D9A-FF03D845A830}" name="Table1" displayName="Table1" ref="A1:C3" totalsRowShown="0" dataDxfId="3">
   <autoFilter ref="A1:C3" xr:uid="{3FB93657-E6D3-447F-9D9A-FF03D845A830}"/>
   <tableColumns count="3">
-    <tableColumn id="3" xr3:uid="{39FAB606-13A9-4181-8A4F-F2D88247E42B}" name="Customer Name (Reference Only)" dataDxfId="4"/>
-    <tableColumn id="1" xr3:uid="{A1381B7C-E420-46E2-B0D0-7022E96A2DB3}" name="Number to Change" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{8653AC77-BA01-49A0-A7F4-6D1004269431}" name="Number to Change To" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{39FAB606-13A9-4181-8A4F-F2D88247E42B}" name="Customer Name (Reference Only)" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{A1381B7C-E420-46E2-B0D0-7022E96A2DB3}" name="Number to Change" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{8653AC77-BA01-49A0-A7F4-6D1004269431}" name="Number to Change To" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -534,9 +534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DB52779-BB51-4D66-9BAF-EF943505CABD}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E2:E6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>